<commit_message>
added trailing LIT sell order
</commit_message>
<xml_diff>
--- a/general/Commision Percantage Calculation.xlsx
+++ b/general/Commision Percantage Calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git Projects\HeikenAshiInvestingModel\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git Projects\HeikenAshiInvestingModel\general\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>commission</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>Minimum value for purshase</t>
+  </si>
+  <si>
+    <t>lose sell sum</t>
+  </si>
+  <si>
+    <t>lose profit</t>
+  </si>
+  <si>
+    <t>Proportion</t>
+  </si>
+  <si>
+    <t>без 2% не очень ,!</t>
   </si>
 </sst>
 </file>
@@ -149,7 +161,19 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -196,24 +220,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G31" totalsRowShown="0" headerRowDxfId="8" dataDxfId="5">
-  <autoFilter ref="A1:G31"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="buy sum USD" dataDxfId="7"/>
-    <tableColumn id="2" name="commission" dataDxfId="6"/>
-    <tableColumn id="3" name="sell sum" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J31" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J31"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="buy sum USD" dataDxfId="9"/>
+    <tableColumn id="2" name="commission" dataDxfId="8"/>
+    <tableColumn id="3" name="sell sum" dataDxfId="0">
       <calculatedColumnFormula>A2*1.005</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="profit " dataDxfId="3">
+    <tableColumn id="4" name="profit " dataDxfId="7">
       <calculatedColumnFormula xml:space="preserve"> C2 -A2-B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="profit percentage" dataDxfId="2">
+    <tableColumn id="5" name="profit percentage" dataDxfId="6">
       <calculatedColumnFormula xml:space="preserve"> D2/A2 *100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="buy sum in AUD" dataDxfId="1">
+    <tableColumn id="6" name="buy sum in AUD" dataDxfId="5">
       <calculatedColumnFormula>A2 *1.5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Comment" dataDxfId="0"/>
+    <tableColumn id="7" name="Comment" dataDxfId="4"/>
+    <tableColumn id="8" name="lose sell sum" dataDxfId="3">
+      <calculatedColumnFormula>A2 * 0.95</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="lose profit" dataDxfId="2">
+      <calculatedColumnFormula>H2-A2 -2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Proportion" dataDxfId="1">
+      <calculatedColumnFormula>I2/D2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,9 +530,12 @@
     <col min="5" max="5" width="24.85546875" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,8 +557,17 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>100</v>
       </c>
@@ -546,8 +591,20 @@
         <v>150</v>
       </c>
       <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="7">
+        <f t="shared" ref="H2:H31" si="4">A2 * 0.95</f>
+        <v>95</v>
+      </c>
+      <c r="I2" s="7">
+        <f t="shared" ref="I2:I31" si="5">H2-A2 -2</f>
+        <v>-7</v>
+      </c>
+      <c r="J2" s="7">
+        <f t="shared" ref="J2:J31" si="6">I2/D2</f>
+        <v>4.6666666666666226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+100</f>
         <v>200</v>
@@ -572,10 +629,22 @@
         <v>300</v>
       </c>
       <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="7">
+        <f t="shared" si="4"/>
+        <v>190</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" si="5"/>
+        <v>-12</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" si="6"/>
+        <v>11.999999999999659</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A10" si="4">A3+100</f>
+        <f t="shared" ref="A4:A10" si="7">A3+100</f>
         <v>300</v>
       </c>
       <c r="B4" s="2">
@@ -598,10 +667,22 @@
         <v>450</v>
       </c>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="7">
+        <f t="shared" si="4"/>
+        <v>285</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="5"/>
+        <v>-17</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="6"/>
+        <v>33.999999999996135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>400</v>
       </c>
       <c r="B5" s="2">
@@ -624,10 +705,22 @@
         <v>600</v>
       </c>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="7">
+        <f t="shared" si="4"/>
+        <v>380</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="5"/>
+        <v>-22</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="6"/>
+        <v>387028092977152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>500</v>
       </c>
       <c r="B6" s="1">
@@ -650,10 +743,22 @@
         <v>750</v>
       </c>
       <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="7">
+        <f t="shared" si="4"/>
+        <v>475</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="5"/>
+        <v>-27</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="6"/>
+        <v>-54.000000000006139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>600</v>
       </c>
       <c r="B7" s="1">
@@ -676,10 +781,22 @@
         <v>900</v>
       </c>
       <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="7">
+        <f t="shared" si="4"/>
+        <v>570</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="5"/>
+        <v>-32</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="6"/>
+        <v>-32.000000000003638</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>700</v>
       </c>
       <c r="B8" s="1">
@@ -702,10 +819,22 @@
         <v>1050</v>
       </c>
       <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="7">
+        <f t="shared" si="4"/>
+        <v>665</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="5"/>
+        <v>-37</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="6"/>
+        <v>-24.666666666668537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>800</v>
       </c>
       <c r="B9" s="5">
@@ -730,10 +859,22 @@
       <c r="G9" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="7">
+        <f t="shared" si="4"/>
+        <v>760</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="5"/>
+        <v>-42</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="6"/>
+        <v>-21.000000000001194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>900</v>
       </c>
       <c r="B10" s="1">
@@ -756,8 +897,20 @@
         <v>1350</v>
       </c>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="7">
+        <f t="shared" si="4"/>
+        <v>855</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="5"/>
+        <v>-47</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="6"/>
+        <v>-18.800000000000853</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>A10+100</f>
         <v>1000</v>
@@ -782,10 +935,22 @@
         <v>1500</v>
       </c>
       <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="7">
+        <f t="shared" si="4"/>
+        <v>950</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="5"/>
+        <v>-52</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="6"/>
+        <v>-17.333333333333989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <f>A11 + 1000</f>
+        <f t="shared" ref="A12:A31" si="8">A11 + 1000</f>
         <v>2000</v>
       </c>
       <c r="B12" s="3">
@@ -810,10 +975,22 @@
       <c r="G12" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="7">
+        <f t="shared" si="4"/>
+        <v>1900</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="5"/>
+        <v>-102</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="6"/>
+        <v>-12.750000000000362</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f>A12 + 1000</f>
+        <f t="shared" si="8"/>
         <v>3000</v>
       </c>
       <c r="B13" s="1">
@@ -836,10 +1013,22 @@
         <v>4500</v>
       </c>
       <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="7">
+        <f t="shared" si="4"/>
+        <v>2850</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="5"/>
+        <v>-152</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="6"/>
+        <v>-11.692307692308102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <f>A13 + 1000</f>
+        <f t="shared" si="8"/>
         <v>4000</v>
       </c>
       <c r="B14" s="6">
@@ -864,10 +1053,22 @@
       <c r="G14" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="7">
+        <f t="shared" si="4"/>
+        <v>3800</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="5"/>
+        <v>-202</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="6"/>
+        <v>-11.222222222222506</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
-        <f>A14 + 1000</f>
+        <f t="shared" si="8"/>
         <v>5000</v>
       </c>
       <c r="B15" s="4">
@@ -890,10 +1091,22 @@
         <v>7500</v>
       </c>
       <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="7">
+        <f t="shared" si="4"/>
+        <v>4750</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="5"/>
+        <v>-252</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.956521739130869</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f>A15 + 1000</f>
+        <f t="shared" si="8"/>
         <v>6000</v>
       </c>
       <c r="B16" s="1">
@@ -916,10 +1129,25 @@
         <v>9000</v>
       </c>
       <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="7">
+        <f t="shared" si="4"/>
+        <v>5700</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="5"/>
+        <v>-302</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.785714285714636</v>
+      </c>
+      <c r="N16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f>A16 + 1000</f>
+        <f t="shared" si="8"/>
         <v>7000</v>
       </c>
       <c r="B17" s="1">
@@ -942,10 +1170,22 @@
         <v>10500</v>
       </c>
       <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="7">
+        <f t="shared" si="4"/>
+        <v>6650</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="5"/>
+        <v>-352</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.666666666666961</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f>A17 + 1000</f>
+        <f t="shared" si="8"/>
         <v>8000</v>
       </c>
       <c r="B18" s="1">
@@ -968,10 +1208,22 @@
         <v>12000</v>
       </c>
       <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="7">
+        <f t="shared" si="4"/>
+        <v>7600</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="5"/>
+        <v>-402</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.578947368421305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f>A18 + 1000</f>
+        <f t="shared" si="8"/>
         <v>9000</v>
       </c>
       <c r="B19" s="1">
@@ -994,10 +1246,22 @@
         <v>13500</v>
       </c>
       <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="7">
+        <f t="shared" si="4"/>
+        <v>8550</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="5"/>
+        <v>-452</v>
+      </c>
+      <c r="J19" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.511627906977189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f>A19 + 1000</f>
+        <f t="shared" si="8"/>
         <v>10000</v>
       </c>
       <c r="B20" s="1">
@@ -1020,10 +1284,22 @@
         <v>15000</v>
       </c>
       <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="7">
+        <f t="shared" si="4"/>
+        <v>9500</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="5"/>
+        <v>-502</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.45833333333373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f>A20 + 1000</f>
+        <f t="shared" si="8"/>
         <v>11000</v>
       </c>
       <c r="B21" s="1">
@@ -1046,10 +1322,22 @@
         <v>16500</v>
       </c>
       <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="7">
+        <f t="shared" si="4"/>
+        <v>10450</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="5"/>
+        <v>-552</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.415094339623</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>A21 + 1000</f>
+        <f t="shared" si="8"/>
         <v>12000</v>
       </c>
       <c r="B22" s="1">
@@ -1072,10 +1360,22 @@
         <v>18000</v>
       </c>
       <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="7">
+        <f t="shared" si="4"/>
+        <v>11400</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="5"/>
+        <v>-602</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.379310344827912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>A22 + 1000</f>
+        <f t="shared" si="8"/>
         <v>13000</v>
       </c>
       <c r="B23" s="1">
@@ -1098,10 +1398,22 @@
         <v>19500</v>
       </c>
       <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="7">
+        <f t="shared" si="4"/>
+        <v>12350</v>
+      </c>
+      <c r="I23" s="7">
+        <f t="shared" si="5"/>
+        <v>-652</v>
+      </c>
+      <c r="J23" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.349206349206648</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>A23 + 1000</f>
+        <f t="shared" si="8"/>
         <v>14000</v>
       </c>
       <c r="B24" s="1">
@@ -1124,10 +1436,22 @@
         <v>21000</v>
       </c>
       <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="7">
+        <f t="shared" si="4"/>
+        <v>13300</v>
+      </c>
+      <c r="I24" s="7">
+        <f t="shared" si="5"/>
+        <v>-702</v>
+      </c>
+      <c r="J24" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.323529411764982</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f>A24 + 1000</f>
+        <f t="shared" si="8"/>
         <v>15000</v>
       </c>
       <c r="B25" s="1">
@@ -1150,10 +1474,22 @@
         <v>22500</v>
       </c>
       <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="7">
+        <f t="shared" si="4"/>
+        <v>14250</v>
+      </c>
+      <c r="I25" s="7">
+        <f t="shared" si="5"/>
+        <v>-752</v>
+      </c>
+      <c r="J25" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.301369863013955</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f>A25 + 1000</f>
+        <f t="shared" si="8"/>
         <v>16000</v>
       </c>
       <c r="B26" s="1">
@@ -1176,10 +1512,22 @@
         <v>24000</v>
       </c>
       <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="7">
+        <f t="shared" si="4"/>
+        <v>15200</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="5"/>
+        <v>-802</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.282051282051523</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f>A26 + 1000</f>
+        <f t="shared" si="8"/>
         <v>17000</v>
       </c>
       <c r="B27" s="1">
@@ -1202,10 +1550,22 @@
         <v>25500</v>
       </c>
       <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="7">
+        <f t="shared" si="4"/>
+        <v>16150</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="5"/>
+        <v>-852</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.265060240963855</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f>A27 + 1000</f>
+        <f t="shared" si="8"/>
         <v>18000</v>
       </c>
       <c r="B28" s="1">
@@ -1228,10 +1588,22 @@
         <v>27000</v>
       </c>
       <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="7">
+        <f t="shared" si="4"/>
+        <v>17100</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="5"/>
+        <v>-902</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.250000000000425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f>A28 + 1000</f>
+        <f t="shared" si="8"/>
         <v>19000</v>
       </c>
       <c r="B29" s="1">
@@ -1254,10 +1626,22 @@
         <v>28500</v>
       </c>
       <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="7">
+        <f t="shared" si="4"/>
+        <v>18050</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="5"/>
+        <v>-952</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.236559139785347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <f>A29 + 1000</f>
+        <f t="shared" si="8"/>
         <v>20000</v>
       </c>
       <c r="B30" s="1">
@@ -1280,10 +1664,22 @@
         <v>30000</v>
       </c>
       <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="7">
+        <f t="shared" si="4"/>
+        <v>19000</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="5"/>
+        <v>-1002</v>
+      </c>
+      <c r="J30" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.224489795918746</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <f>A30 + 1000</f>
+        <f t="shared" si="8"/>
         <v>21000</v>
       </c>
       <c r="B31" s="1">
@@ -1306,6 +1702,18 @@
         <v>31500</v>
       </c>
       <c r="G31" s="7"/>
+      <c r="H31" s="7">
+        <f t="shared" si="4"/>
+        <v>19950</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="5"/>
+        <v>-1052</v>
+      </c>
+      <c r="J31" s="7">
+        <f t="shared" si="6"/>
+        <v>-10.21359223301007</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E31">

</xml_diff>